<commit_message>
Read users from Excel
</commit_message>
<xml_diff>
--- a/src/main/resources/test_users.xlsx
+++ b/src/main/resources/test_users.xlsx
@@ -16,12 +16,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Sandro</t>
   </si>
   <si>
     <t>Brändli</t>
+  </si>
+  <si>
+    <t>Vorname</t>
+  </si>
+  <si>
+    <t>Nachname</t>
+  </si>
+  <si>
+    <t>Karte</t>
   </si>
 </sst>
 </file>
@@ -360,22 +369,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C2">
         <v>12345</v>
       </c>
     </row>

</xml_diff>